<commit_message>
Fixed search engine data
</commit_message>
<xml_diff>
--- a/data/main_survey_relabelled.xlsx
+++ b/data/main_survey_relabelled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\Documents\Aberdeen\MSc_AI\CS5063_Evaluation_of_AI_systems\assessment\assessment2\eval_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA41CA95-970E-486B-92CB-6EC100A99552}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D135000-CE9F-4331-83EC-3B0906D03B45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6890C1C3-7E71-4571-8028-CDF0E2DD6676}"/>
   </bookViews>
@@ -180,9 +180,6 @@
     <t>Life Sciences and Medicine</t>
   </si>
   <si>
-    <t>Yahoo;Bing;DuckDuckGo</t>
-  </si>
-  <si>
     <t>maillard reaction</t>
   </si>
   <si>
@@ -250,9 +247,6 @@
   </si>
   <si>
     <t>Speed and layout</t>
-  </si>
-  <si>
-    <t>Yahoo;Bing;Ecosia</t>
   </si>
   <si>
     <t>Star Wars Han Solo Christmas Coffee Mug</t>
@@ -477,67 +471,73 @@
     <t xml:space="preserve">the survey presentation can be improved . </t>
   </si>
   <si>
+    <t>adobe</t>
+  </si>
+  <si>
+    <t>I liked the wide range of different web sites it referred me to.</t>
+  </si>
+  <si>
+    <t>the logo</t>
+  </si>
+  <si>
+    <t>Consent</t>
+  </si>
+  <si>
+    <t>What is your gender?</t>
+  </si>
+  <si>
+    <t>What field do you study in?</t>
+  </si>
+  <si>
+    <t>Which search engine do you normally use?</t>
+  </si>
+  <si>
+    <t>Which search engines have you used before?</t>
+  </si>
+  <si>
+    <t>Web search results relevance - Google</t>
+  </si>
+  <si>
+    <t>Web search results relevance - Yippy</t>
+  </si>
+  <si>
+    <t>Image search results relevance - Google</t>
+  </si>
+  <si>
+    <t>Image search results relevance - Yippy</t>
+  </si>
+  <si>
+    <t>Video search results relevance - Google</t>
+  </si>
+  <si>
+    <t>Video search results relevance - Yippy</t>
+  </si>
+  <si>
+    <t>News search results relevance - Google</t>
+  </si>
+  <si>
+    <t>News search results relevance - Yippy</t>
+  </si>
+  <si>
+    <t>Yippy clustering feature - how relevant were the topics?</t>
+  </si>
+  <si>
+    <t>Yippy clustering feature - how useful did you find it?</t>
+  </si>
+  <si>
+    <t>How would you rate the speed of the search?</t>
+  </si>
+  <si>
+    <t>How much do you prefer Google over Yippy?</t>
+  </si>
+  <si>
+    <t>Yahoo;Bing;DuckDuckGo</t>
+  </si>
+  <si>
+    <t>Yahoo;Bing;Ecosia</t>
+  </si>
+  <si>
     <t>Bing</t>
-  </si>
-  <si>
-    <t>adobe</t>
-  </si>
-  <si>
-    <t>I liked the wide range of different web sites it referred me to.</t>
-  </si>
-  <si>
-    <t>the logo</t>
-  </si>
-  <si>
-    <t>Consent</t>
-  </si>
-  <si>
-    <t>What is your gender?</t>
-  </si>
-  <si>
-    <t>What field do you study in?</t>
-  </si>
-  <si>
-    <t>Which search engine do you normally use?</t>
-  </si>
-  <si>
-    <t>Which search engines have you used before?</t>
-  </si>
-  <si>
-    <t>Web search results relevance - Google</t>
-  </si>
-  <si>
-    <t>Web search results relevance - Yippy</t>
-  </si>
-  <si>
-    <t>Image search results relevance - Google</t>
-  </si>
-  <si>
-    <t>Image search results relevance - Yippy</t>
-  </si>
-  <si>
-    <t>Video search results relevance - Google</t>
-  </si>
-  <si>
-    <t>Video search results relevance - Yippy</t>
-  </si>
-  <si>
-    <t>News search results relevance - Google</t>
-  </si>
-  <si>
-    <t>News search results relevance - Yippy</t>
-  </si>
-  <si>
-    <t>Yippy clustering feature - how relevant were the topics?</t>
-  </si>
-  <si>
-    <t>Yippy clustering feature - how useful did you find it?</t>
-  </si>
-  <si>
-    <t>How would you rate the speed of the search?</t>
-  </si>
-  <si>
-    <t>How much do you prefer Google over Yippy?</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49DDDBC-6C51-444E-8552-5A3D9BE7B44A}">
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1054,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1063,16 +1063,16 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" t="s">
         <v>148</v>
-      </c>
-      <c r="F1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H1" t="s">
-        <v>151</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
@@ -1081,43 +1081,43 @@
         <v>4</v>
       </c>
       <c r="K1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M1" t="s">
+        <v>151</v>
+      </c>
+      <c r="N1" t="s">
         <v>152</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>153</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>154</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>155</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>156</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>157</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>158</v>
-      </c>
-      <c r="R1" t="s">
-        <v>159</v>
-      </c>
-      <c r="S1" t="s">
-        <v>160</v>
-      </c>
-      <c r="T1" t="s">
-        <v>161</v>
       </c>
       <c r="U1" t="s">
         <v>5</v>
       </c>
       <c r="V1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="W1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="X1" t="s">
         <v>6</v>
@@ -1160,7 +1160,7 @@
       <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -1249,7 +1249,7 @@
       <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1338,7 +1338,7 @@
       <c r="G4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>32</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1427,7 +1427,7 @@
       <c r="G5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1516,7 +1516,7 @@
       <c r="G6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
         <v>25</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1605,14 +1605,14 @@
       <c r="G7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" t="s">
+        <v>161</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="K7">
         <v>10</v>
@@ -1654,10 +1654,10 @@
         <v>9</v>
       </c>
       <c r="X7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y7" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="Z7">
         <v>2</v>
@@ -1694,14 +1694,14 @@
       <c r="G8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="K8">
         <v>10</v>
@@ -1743,10 +1743,10 @@
         <v>5</v>
       </c>
       <c r="X8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y8" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="Z8">
         <v>6</v>
@@ -1772,7 +1772,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>15</v>
@@ -1781,16 +1781,16 @@
         <v>24</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="K9">
         <v>9</v>
@@ -1832,22 +1832,22 @@
         <v>5</v>
       </c>
       <c r="X9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y9" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="Z9">
         <v>1</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB9">
         <v>6</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
@@ -1861,25 +1861,25 @@
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" t="s">
         <v>25</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K10">
         <v>9</v>
@@ -1921,10 +1921,10 @@
         <v>6</v>
       </c>
       <c r="X10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y10" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="Z10">
         <v>10</v>
@@ -1961,14 +1961,14 @@
       <c r="G11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" t="s">
         <v>25</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K11">
         <v>9</v>
@@ -2010,10 +2010,10 @@
         <v>6</v>
       </c>
       <c r="X11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y11" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="Y11" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="Z11">
         <v>8</v>
@@ -2050,14 +2050,14 @@
       <c r="G12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>69</v>
+      <c r="H12" t="s">
+        <v>162</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K12">
         <v>6</v>
@@ -2099,10 +2099,10 @@
         <v>7</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Z12">
         <v>6</v>
@@ -2139,14 +2139,14 @@
       <c r="G13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>73</v>
+      <c r="H13" t="s">
+        <v>71</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K13">
         <v>10</v>
@@ -2191,7 +2191,7 @@
         <v>20</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Z13">
         <v>1</v>
@@ -2228,14 +2228,14 @@
       <c r="G14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>76</v>
+      <c r="H14" t="s">
+        <v>74</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K14">
         <v>9</v>
@@ -2277,10 +2277,10 @@
         <v>9</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Z14">
         <v>3</v>
@@ -2292,7 +2292,7 @@
         <v>9</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
@@ -2306,7 +2306,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>30</v>
@@ -2317,14 +2317,14 @@
       <c r="G15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>82</v>
+      <c r="H15" t="s">
+        <v>80</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K15">
         <v>10</v>
@@ -2366,10 +2366,10 @@
         <v>2</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Z15">
         <v>2</v>
@@ -2395,7 +2395,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>30</v>
@@ -2406,14 +2406,14 @@
       <c r="G16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>86</v>
+      <c r="H16" t="s">
+        <v>84</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K16">
         <v>9</v>
@@ -2455,16 +2455,16 @@
         <v>10</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Z16">
         <v>3</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AB16">
         <v>7</v>
@@ -2495,14 +2495,14 @@
       <c r="G17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" t="s">
         <v>17</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K17">
         <v>6</v>
@@ -2544,22 +2544,22 @@
         <v>9</v>
       </c>
       <c r="X17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z17">
+        <v>9</v>
+      </c>
+      <c r="AA17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="Y17" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z17">
-        <v>9</v>
-      </c>
-      <c r="AA17" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="AB17">
         <v>10</v>
       </c>
       <c r="AC17" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
@@ -2573,7 +2573,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>30</v>
@@ -2584,14 +2584,14 @@
       <c r="G18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>95</v>
+      <c r="H18" t="s">
+        <v>93</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K18">
         <v>9</v>
@@ -2633,10 +2633,10 @@
         <v>10</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Z18">
         <v>2</v>
@@ -2648,7 +2648,7 @@
         <v>8</v>
       </c>
       <c r="AC18" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
@@ -2662,7 +2662,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>15</v>
@@ -2673,59 +2673,59 @@
       <c r="G19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19">
+        <v>8</v>
+      </c>
+      <c r="L19">
+        <v>8</v>
+      </c>
+      <c r="M19">
+        <v>9</v>
+      </c>
+      <c r="N19">
+        <v>8</v>
+      </c>
+      <c r="O19">
+        <v>9</v>
+      </c>
+      <c r="P19">
+        <v>9</v>
+      </c>
+      <c r="Q19">
+        <v>9</v>
+      </c>
+      <c r="R19">
+        <v>9</v>
+      </c>
+      <c r="S19">
+        <v>9</v>
+      </c>
+      <c r="T19">
+        <v>8</v>
+      </c>
+      <c r="U19">
+        <v>9</v>
+      </c>
+      <c r="V19">
+        <v>9</v>
+      </c>
+      <c r="W19">
+        <v>9</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y19" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="K19">
-        <v>8</v>
-      </c>
-      <c r="L19">
-        <v>8</v>
-      </c>
-      <c r="M19">
-        <v>9</v>
-      </c>
-      <c r="N19">
-        <v>8</v>
-      </c>
-      <c r="O19">
-        <v>9</v>
-      </c>
-      <c r="P19">
-        <v>9</v>
-      </c>
-      <c r="Q19">
-        <v>9</v>
-      </c>
-      <c r="R19">
-        <v>9</v>
-      </c>
-      <c r="S19">
-        <v>9</v>
-      </c>
-      <c r="T19">
-        <v>8</v>
-      </c>
-      <c r="U19">
-        <v>9</v>
-      </c>
-      <c r="V19">
-        <v>9</v>
-      </c>
-      <c r="W19">
-        <v>9</v>
-      </c>
-      <c r="X19" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y19" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="Z19">
         <v>9</v>
@@ -2762,14 +2762,14 @@
       <c r="G20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>95</v>
+      <c r="H20" t="s">
+        <v>93</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K20">
         <v>10</v>
@@ -2811,10 +2811,10 @@
         <v>10</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Z20">
         <v>1</v>
@@ -2840,7 +2840,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>30</v>
@@ -2849,16 +2849,16 @@
         <v>44</v>
       </c>
       <c r="G21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" t="s">
+        <v>105</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="K21">
         <v>7</v>
@@ -2900,10 +2900,10 @@
         <v>5</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Z21">
         <v>8</v>
@@ -2929,10 +2929,10 @@
         <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>24</v>
@@ -2940,14 +2940,14 @@
       <c r="G22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>95</v>
+      <c r="H22" t="s">
+        <v>93</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K22">
         <v>9</v>
@@ -3029,14 +3029,14 @@
       <c r="G23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>113</v>
+      <c r="H23" t="s">
+        <v>111</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K23">
         <v>10</v>
@@ -3078,10 +3078,10 @@
         <v>8</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Y23" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Z23">
         <v>2</v>
@@ -3118,14 +3118,14 @@
       <c r="G24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>95</v>
+      <c r="H24" t="s">
+        <v>93</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K24">
         <v>9</v>
@@ -3167,10 +3167,10 @@
         <v>10</v>
       </c>
       <c r="X24" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Y24" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Z24">
         <v>1</v>
@@ -3207,14 +3207,14 @@
       <c r="G25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>120</v>
+      <c r="H25" t="s">
+        <v>118</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K25">
         <v>8</v>
@@ -3256,10 +3256,10 @@
         <v>10</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Y25" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Z25">
         <v>1</v>
@@ -3296,71 +3296,71 @@
       <c r="G26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>82</v>
+      <c r="H26" t="s">
+        <v>80</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J26" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="K26">
+        <v>9</v>
+      </c>
+      <c r="L26">
+        <v>9</v>
+      </c>
+      <c r="M26">
+        <v>9</v>
+      </c>
+      <c r="N26">
+        <v>8</v>
+      </c>
+      <c r="O26">
+        <v>9</v>
+      </c>
+      <c r="P26">
+        <v>8</v>
+      </c>
+      <c r="Q26">
+        <v>9</v>
+      </c>
+      <c r="R26">
+        <v>9</v>
+      </c>
+      <c r="S26">
+        <v>10</v>
+      </c>
+      <c r="T26">
+        <v>10</v>
+      </c>
+      <c r="U26">
+        <v>9</v>
+      </c>
+      <c r="V26">
+        <v>9</v>
+      </c>
+      <c r="W26">
+        <v>7</v>
+      </c>
+      <c r="X26" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y26" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="K26">
-        <v>9</v>
-      </c>
-      <c r="L26">
-        <v>9</v>
-      </c>
-      <c r="M26">
-        <v>9</v>
-      </c>
-      <c r="N26">
-        <v>8</v>
-      </c>
-      <c r="O26">
-        <v>9</v>
-      </c>
-      <c r="P26">
-        <v>8</v>
-      </c>
-      <c r="Q26">
-        <v>9</v>
-      </c>
-      <c r="R26">
-        <v>9</v>
-      </c>
-      <c r="S26">
-        <v>10</v>
-      </c>
-      <c r="T26">
-        <v>10</v>
-      </c>
-      <c r="U26">
-        <v>9</v>
-      </c>
-      <c r="V26">
-        <v>9</v>
-      </c>
-      <c r="W26">
-        <v>7</v>
-      </c>
-      <c r="X26" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="Y26" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="Z26">
         <v>4</v>
       </c>
       <c r="AA26" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AB26">
         <v>10</v>
       </c>
       <c r="AC26" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
@@ -3385,14 +3385,14 @@
       <c r="G27" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" t="s">
         <v>25</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K27">
         <v>8</v>
@@ -3434,10 +3434,10 @@
         <v>5</v>
       </c>
       <c r="X27" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y27" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Z27">
         <v>5</v>
@@ -3474,14 +3474,14 @@
       <c r="G28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" t="s">
         <v>25</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K28">
         <v>9</v>
@@ -3563,14 +3563,14 @@
       <c r="G29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>73</v>
+      <c r="H29" t="s">
+        <v>71</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K29">
         <v>8</v>
@@ -3612,10 +3612,10 @@
         <v>7</v>
       </c>
       <c r="X29" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Y29" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Z29">
         <v>3</v>
@@ -3652,14 +3652,14 @@
       <c r="G30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>106</v>
+      <c r="H30" t="s">
+        <v>104</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K30">
         <v>8</v>
@@ -3701,10 +3701,10 @@
         <v>8</v>
       </c>
       <c r="X30" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Y30" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Z30">
         <v>6</v>
@@ -3730,7 +3730,7 @@
         <v>13</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>30</v>
@@ -3741,14 +3741,14 @@
       <c r="G31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" t="s">
         <v>25</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K31">
         <v>5</v>
@@ -3790,22 +3790,22 @@
         <v>8</v>
       </c>
       <c r="X31" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y31" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z31">
+        <v>7</v>
+      </c>
+      <c r="AA31" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="Y31" s="2" t="s">
+      <c r="AB31">
+        <v>8</v>
+      </c>
+      <c r="AC31" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="Z31">
-        <v>7</v>
-      </c>
-      <c r="AA31" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB31">
-        <v>8</v>
-      </c>
-      <c r="AC31" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
@@ -3819,7 +3819,7 @@
         <v>23</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>30</v>
@@ -3830,14 +3830,14 @@
       <c r="G32" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>143</v>
+      <c r="H32" t="s">
+        <v>163</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K32">
         <v>6</v>
@@ -3879,10 +3879,10 @@
         <v>8</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="Y32" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="Z32">
         <v>8</v>

</xml_diff>